<commit_message>
[IMP] Points in previous commit, Some cleanup on constants
</commit_message>
<xml_diff>
--- a/stock_orderpoint_impex_matrix/tests/fixtures/delete_wh1_product27_product11.xlsx
+++ b/stock_orderpoint_impex_matrix/tests/fixtures/delete_wh1_product27_product11.xlsx
@@ -31,6 +31,12 @@
     <t xml:space="preserve">Article</t>
   </si>
   <si>
+    <t xml:space="preserve">Multiple de quantité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Délai fournisseur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantité actuelle</t>
   </si>
   <si>
@@ -40,19 +46,13 @@
     <t xml:space="preserve">Quantité maximale</t>
   </si>
   <si>
-    <t xml:space="preserve">Délai fournisseur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple de quantité</t>
-  </si>
-  <si>
     <t xml:space="preserve">E-COM12</t>
   </si>
   <si>
     <t xml:space="preserve">Conference Chair</t>
   </si>
   <si>
-    <t xml:space="preserve">FURN_8900</t>
+    <t xml:space="preserve">FURN_8855</t>
   </si>
   <si>
     <t xml:space="preserve">Drawer</t>
@@ -165,11 +165,14 @@
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="6" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="12" min="11" style="0" width="13.02"/>
   </cols>
   <sheetData>

</xml_diff>